<commit_message>
updated 2.1 silver review change list
</commit_message>
<xml_diff>
--- a/implementation/caarray_silver_compatibility_review/2.1/required_changes.xlsx
+++ b/implementation/caarray_silver_compatibility_review/2.1/required_changes.xlsx
@@ -24,6 +24,424 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="138">
   <si>
+    <t>The UML definition of two classes "IntegerColumn" and "LongColumn" are same, ""Contains integral data values of a specific quantitation type for a single microarray hybridization." ".  Suggested defin (LongColumn) [Shantanu Deshpande]</t>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UML entities should have a defined, concrete meaning (not be abstract).</t>
+  </si>
+  <si>
+    <t>very abstract (Category) [Quan Chen]</t>
+  </si>
+  <si>
+    <t>No comment (StringColumn) [Xin Zheng]</t>
+  </si>
+  <si>
+    <t>Best Practices - Classes and Attributes</t>
+  </si>
+  <si>
+    <t>The concepts assigned to each class and attribute must be synonymous (consistent) with the developer-derived UML definition.</t>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subtype</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subtype Description</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes/No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Declined?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolution</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">check the source side *..* ([Term-TermSource]) [Xin Zheng] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Models</t>
+  </si>
+  <si>
+    <t>Best Practices - Associations</t>
+  </si>
+  <si>
+    <t>Association ends must explicitly define multiplicity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are multiplicities of *..* for both ends what is desired? ([Person-Organization]) [Grace Stafford] </t>
+  </si>
+  <si>
+    <t>But the source side might be wrong ([Term-Category]) [Xin Zheng]</t>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The names given to packages, classes, and attributes should accurately convey their meaning (as determined by the UML definition).  In other words, the name should be consistent with the definition.</t>
+  </si>
+  <si>
+    <t>The definition is consistent with the class.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rework definition to include concept of caArray (AbstractCaArrayEntity) [Becky Boes]</t>
+  </si>
+  <si>
+    <t>The definition does not convey the same meaning as the class name. (AbstractDesignElement) [Becky Boes]</t>
+  </si>
+  <si>
+    <t>The UML definitions for the classes and attributes ccurately describe what they represent and are sufficiently clear to enable accurate semantic annotation.</t>
+  </si>
+  <si>
+    <t>The UML definition is "The ordered textual data values for the column. That may not be clear enough for concept mapping. (gov.nih.nci.caarray.domain.data.StringColumn.values) [Xin Zheng]</t>
+  </si>
+  <si>
+    <t>Order_Value may not be the best mapping (gov.nih.nci.caarray.domain.data.StringColumn.values) [Xin Zheng]</t>
+  </si>
+  <si>
+    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidObjectId) [Salvatore Mungal]</t>
+  </si>
+  <si>
+    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidNamespace) [Salvatore Mungal]</t>
+  </si>
+  <si>
+    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidAuthority) [Salvatore Mungal]</t>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>concepts do not match UML definition - definition does not include caArray (AbstractCaArrayEntity) [Becky Boes]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this mapping does not reflect the ontology part of the UML definition (TermBasedCharacteristic) [Xin Zheng] </t>
+  </si>
+  <si>
+    <t>It is mapped to Tracer_Nucleic Acids. This need to be double checked. (LabeledExtract) [Xin Zheng]</t>
+  </si>
+  <si>
+    <t>The UML definitions for the Classes and attributes accurately describe what they represent and are sufficiently clear to enable accurate semantic annotation.</t>
+  </si>
+  <si>
+    <t>YELLOW: Criteria that are suggested.  These criteria improve interoperability but it is not absolutely required that they be met.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will update definition</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update concepts with something that encompasses both person and org</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update concept(s) to better match definition</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Term" concept covers the ontology</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>The concepts do not include the idea of "report a quantified value" but the definition does. (AbstractDesignElement) [Becky Boes]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Practices - Naming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Practices - Naming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The class name does not convey the same meaning as the description. (AbstractDesignElement) [Becky Boes] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Practices - Modeling</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Practices - Modeling</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Person</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Term</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExperimentContact</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbstractContact</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbstractDesignElement</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringColumn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbstractCaArrayEntity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TermBasedCharacteristic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LabeledExtract</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LongColumn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbstractProbeAnnotation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Publication</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes/No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rework definition for clarity.  The concept of \"given array reporter\" is not clear. The class name and concepts include \"Annotation\" but it is not included in the definition. (AbstractProbeAnnotation) [Becky Boes]</t>
+  </si>
+  <si>
+    <t>note-"article" misspelled (Publication) [Grace Stafford]</t>
+  </si>
+  <si>
     <t>Concept contactPerson does not include the notion of a "party" or "organization". (AbstractContact) [Becky Boes]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -108,10 +526,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>It is clear enough</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Will update definitions to include precision of data type; also applies to double/float, long/short</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -134,432 +548,12 @@
   <si>
     <t>RED: Criteria that are absolutely required for compatibility</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>YELLOW: Criteria that are suggested.  These criteria improve interoperability but it is not absolutely required that they be met.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Will update definition</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update concepts with something that encompasses both person and org</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update concept(s) to better match definition</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Term" concept covers the ontology</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The concepts do not include the idea of "report a quantified value" but the definition does. (AbstractDesignElement) [Becky Boes]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best Practices - Naming</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best Practices - Naming</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The class name does not convey the same meaning as the description. (AbstractDesignElement) [Becky Boes] </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best Practices - Modeling</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best Practices - Modeling</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Person</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Term</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExperimentContact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AbstractContact</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AbstractDesignElement</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Category</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>StringColumn</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AbstractCaArrayEntity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TermBasedCharacteristic</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LabeledExtract</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LongColumn</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AbstractProbeAnnotation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Publication</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes/No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rework definition for clarity.  The concept of \"given array reporter\" is not clear. The class name and concepts include \"Annotation\" but it is not included in the definition. (AbstractProbeAnnotation) [Becky Boes]</t>
-  </si>
-  <si>
-    <t>note-"article" misspelled (Publication) [Grace Stafford]</t>
-  </si>
-  <si>
-    <t>Rework definition to include concept of caArray (AbstractCaArrayEntity) [Becky Boes]</t>
-  </si>
-  <si>
-    <t>The definition does not convey the same meaning as the class name. (AbstractDesignElement) [Becky Boes]</t>
-  </si>
-  <si>
-    <t>The UML definitions for the classes and attributes ccurately describe what they represent and are sufficiently clear to enable accurate semantic annotation.</t>
-  </si>
-  <si>
-    <t>The UML definition is "The ordered textual data values for the column. That may not be clear enough for concept mapping. (gov.nih.nci.caarray.domain.data.StringColumn.values) [Xin Zheng]</t>
-  </si>
-  <si>
-    <t>Order_Value may not be the best mapping (gov.nih.nci.caarray.domain.data.StringColumn.values) [Xin Zheng]</t>
-  </si>
-  <si>
-    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidObjectId) [Salvatore Mungal]</t>
-  </si>
-  <si>
-    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidNamespace) [Salvatore Mungal]</t>
-  </si>
-  <si>
-    <t>The concept "Part" should be left out in the next iteration. (gov.nih.nci.caarray.domain.project.Factor.lsidAuthority) [Salvatore Mungal]</t>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>concepts do not match UML definition - definition does not include caArray (AbstractCaArrayEntity) [Becky Boes]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this mapping does not reflect the ontology part of the UML definition (TermBasedCharacteristic) [Xin Zheng] </t>
-  </si>
-  <si>
-    <t>It is mapped to Tracer_Nucleic Acids. This need to be double checked. (LabeledExtract) [Xin Zheng]</t>
-  </si>
-  <si>
-    <t>The UML definitions for the Classes and attributes accurately describe what they represent and are sufficiently clear to enable accurate semantic annotation.</t>
-  </si>
-  <si>
-    <t>The UML definition of two classes "IntegerColumn" and "LongColumn" are same, ""Contains integral data values of a specific quantitation type for a single microarray hybridization." ".  Suggested defin (LongColumn) [Shantanu Deshpande]</t>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UML entities should have a defined, concrete meaning (not be abstract).</t>
-  </si>
-  <si>
-    <t>very abstract (Category) [Quan Chen]</t>
-  </si>
-  <si>
-    <t>No comment (StringColumn) [Xin Zheng]</t>
-  </si>
-  <si>
-    <t>Best Practices - Classes and Attributes</t>
-  </si>
-  <si>
-    <t>The concepts assigned to each class and attribute must be synonymous (consistent) with the developer-derived UML definition.</t>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Subtype</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Subtype Description</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes/No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Issue</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Declined?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resolution</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">check the source side *..* ([Term-TermSource]) [Xin Zheng] </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information Models</t>
-  </si>
-  <si>
-    <t>Best Practices - Associations</t>
-  </si>
-  <si>
-    <t>Association ends must explicitly define multiplicity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are multiplicities of *..* for both ends what is desired? ([Person-Organization]) [Grace Stafford] </t>
-  </si>
-  <si>
-    <t>But the source side might be wrong ([Term-Category]) [Xin Zheng]</t>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>The names given to packages, classes, and attributes should accurately convey their meaning (as determined by the UML definition).  In other words, the name should be consistent with the definition.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -990,10 +984,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1012,849 +1006,849 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="13" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="6" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A8" s="2" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="39">
       <c r="A11" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="52">
       <c r="A12" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="52">
       <c r="A13" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="26">
       <c r="A14" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="H14" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="26">
       <c r="A15" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="39">
       <c r="A16" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39">
       <c r="A17" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="39">
       <c r="A18" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="39">
       <c r="A19" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="39">
       <c r="A20" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="39">
       <c r="A21" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="H21" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="39">
       <c r="A22" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="10" customFormat="1" ht="52">
       <c r="A23" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="52">
       <c r="A24" s="11" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="52">
       <c r="A25" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G25" s="6" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="52">
       <c r="A26" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="52">
       <c r="A27" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="I27" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="52">
       <c r="A28" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="52">
       <c r="A29" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="H29" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="52">
       <c r="A30" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="39">
       <c r="A31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="26">
       <c r="A32" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="26">
       <c r="A33" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="26">
       <c r="A34" s="7" t="s">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1892,12 +1886,11 @@
     <row r="42" spans="1:9">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:9" ht="26"/>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <autoFilter ref="A7:J34"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>